<commit_message>
modified code to move universal prams into universal params excel sheet; also modifying various scripts to output expected paper figures better
</commit_message>
<xml_diff>
--- a/UniversalParams.xlsx
+++ b/UniversalParams.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnwen/JohnCode/mord/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/keimasuda/Desktop/JohnKeiNPAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB5FED9-E128-F044-AB3F-331796403D76}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{796D402B-0681-614E-9435-93E7DBCD06E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="21580" windowHeight="8060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="45460" windowHeight="10760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,20 +28,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>SpeedCutoff</t>
   </si>
   <si>
-    <t>InFieldThreshold</t>
-  </si>
-  <si>
-    <t>OutFieldThreshold</t>
-  </si>
-  <si>
-    <t>FieldExtensionThreshold</t>
-  </si>
-  <si>
     <t>TrackStart</t>
   </si>
   <si>
@@ -57,29 +48,32 @@
     <t>SmoothSigmaFR</t>
   </si>
   <si>
-    <t>WorkingDirectory</t>
-  </si>
-  <si>
-    <t>CellFileName</t>
-  </si>
-  <si>
-    <t>Cells_ContrastExperiment.xlsx</t>
-  </si>
-  <si>
-    <t>Z:\Projects\ContrastExperiment\</t>
+    <t>LargerSpatialBin</t>
+  </si>
+  <si>
+    <t>trials_corrTemplate</t>
+  </si>
+  <si>
+    <t>ds_factor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -102,8 +96,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,85 +379,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="6" width="9" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" customWidth="1"/>
+    <col min="4" max="4" width="9" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" customWidth="1"/>
+    <col min="8" max="8" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0.02</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>400</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="H2">
+        <v>50</v>
+      </c>
+      <c r="I2">
         <v>1</v>
-      </c>
-      <c r="I1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2">
-        <v>0.02</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>320</v>
-      </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
-      <c r="H2">
-        <v>85</v>
-      </c>
-      <c r="I2">
-        <v>5</v>
-      </c>
-      <c r="J2">
-        <v>70</v>
-      </c>
-      <c r="K2">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed timewarmping code so that it actually time warps each cells score based on its session; added some hard coded numbers to universal params excel spreadsheet
</commit_message>
<xml_diff>
--- a/UniversalParams.xlsx
+++ b/UniversalParams.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/keimasuda/Desktop/JohnKeiNPAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{796D402B-0681-614E-9435-93E7DBCD06E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{050037EF-9D22-F349-9D65-F5A6A8EC2C84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="45460" windowHeight="10760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>SpeedCutoff</t>
   </si>
@@ -55,6 +55,15 @@
   </si>
   <si>
     <t>ds_factor</t>
+  </si>
+  <si>
+    <t>ketamineTrial</t>
+  </si>
+  <si>
+    <t>controlTrial</t>
+  </si>
+  <si>
+    <t>gainTrial</t>
   </si>
 </sst>
 </file>
@@ -379,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -395,7 +404,7 @@
     <col min="8" max="8" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -423,8 +432,17 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0.02</v>
       </c>
@@ -450,7 +468,16 @@
         <v>50</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>100</v>
+      </c>
+      <c r="J2">
+        <v>100</v>
+      </c>
+      <c r="K2">
+        <v>50</v>
+      </c>
+      <c r="L2">
+        <v>290</v>
       </c>
     </row>
   </sheetData>

</xml_diff>